<commit_message>
Added Plakat PowerPoint (empty) and updated gitignore for Mac.
</commit_message>
<xml_diff>
--- a/Dokumentation/arbeitszeiten/Arbeitszeiten_scd42636.xlsx
+++ b/Dokumentation/arbeitszeiten/Arbeitszeiten_scd42636.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dominik/Documents/Schule/Hochschule/IT7/DT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dominik/Documents/Schule/Hochschule/IT7/DT/git/DT_WS1718_02_StarCar/Dokumentation/arbeitszeiten/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" tabRatio="933"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" tabRatio="933" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung" sheetId="13" r:id="rId1"/>
@@ -225,7 +225,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="229">
+  <cellStyleXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -455,8 +455,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -492,11 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -514,15 +513,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -530,8 +520,26 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="229">
+  <cellStyles count="233">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -646,6 +654,8 @@
     <cellStyle name="Besuchter Link" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -760,9 +770,11 @@
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="55">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -865,6 +877,86 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1230,436 +1322,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1997,7 +1659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2020,11 +1682,11 @@
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
@@ -2035,7 +1697,7 @@
       <c r="B4" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -2046,12 +1708,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33">
+      <c r="A7" s="30">
         <v>43009</v>
       </c>
       <c r="B7" s="2">
         <f>'Oktober 2017'!G34</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <f>'Oktober 2017'!C33</f>
@@ -2059,7 +1721,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="33">
+      <c r="A8" s="30">
         <v>43040</v>
       </c>
       <c r="B8" s="2">
@@ -2072,7 +1734,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="33">
+      <c r="A9" s="30">
         <v>43070</v>
       </c>
       <c r="B9" s="2">
@@ -2085,7 +1747,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="33">
+      <c r="A10" s="30">
         <v>43101</v>
       </c>
       <c r="B10" s="2">
@@ -2098,7 +1760,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
@@ -2108,7 +1770,7 @@
       </c>
       <c r="B12" s="2">
         <f>SUM(B7:B9)</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <f>SUM(C7:C10)</f>
@@ -2146,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2163,7 +1825,7 @@
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2189,142 +1851,142 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39">
+    <row r="2" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36">
         <f>DATE(2017,10,1)</f>
         <v>43009</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="31">
         <f>A2</f>
         <v>43009</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="32">
         <f>WEEKNUM(A2,2)</f>
         <v>40</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34">
         <f>(E2-D2-F2)*24</f>
         <v>0</v>
       </c>
-      <c r="H2" s="37"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="39">
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="36">
         <f>A2+1</f>
         <v>43010</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="31">
         <f t="shared" ref="B3:B32" si="0">A3</f>
         <v>43010</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="32">
         <f t="shared" ref="C3:C32" si="1">WEEKNUM(A3,2)</f>
         <v>41</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37">
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34">
         <f t="shared" ref="G3:G32" si="2">(E3-D3-F3)*24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="39">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="36">
         <f t="shared" ref="A4:A32" si="3">A3+1</f>
         <v>43011</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="31">
         <f t="shared" si="0"/>
         <v>43011</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="32">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="39">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
         <f t="shared" si="3"/>
         <v>43012</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="31">
         <f t="shared" si="0"/>
         <v>43012</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="32">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="39">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="36">
         <f t="shared" si="3"/>
         <v>43013</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="32">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46">
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="40">
         <f t="shared" si="3"/>
         <v>43014</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="41">
         <f t="shared" si="0"/>
         <v>43014</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="42">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="43">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="43">
         <v>0.57291666666666663</v>
       </c>
-      <c r="F7" s="49">
-        <v>0</v>
-      </c>
-      <c r="G7" s="50">
+      <c r="F7" s="43">
+        <v>0</v>
+      </c>
+      <c r="G7" s="44">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="H7" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <f t="shared" si="3"/>
         <v>43015</v>
@@ -2346,7 +2008,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <f t="shared" si="3"/>
         <v>43016</v>
@@ -2368,7 +2030,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <f t="shared" si="3"/>
         <v>43017</v>
@@ -2389,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <f t="shared" si="3"/>
         <v>43018</v>
@@ -2410,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <f t="shared" si="3"/>
         <v>43019</v>
@@ -2431,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
         <f t="shared" si="3"/>
         <v>43020</v>
@@ -2452,27 +2114,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40">
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37">
         <f t="shared" si="3"/>
         <v>43021</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="38">
         <f t="shared" si="0"/>
         <v>43021</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="39">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="43">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E14" s="43">
+        <v>0.59375</v>
+      </c>
+      <c r="F14" s="43">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5000000000000004</v>
+      </c>
+      <c r="H14" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
         <f t="shared" si="3"/>
         <v>43022</v>
@@ -2494,7 +2169,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
         <f t="shared" si="3"/>
         <v>43023</v>
@@ -2516,7 +2191,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <f t="shared" si="3"/>
         <v>43024</v>
@@ -2529,16 +2204,22 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="D17" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
       <c r="G17" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
         <f t="shared" si="3"/>
         <v>43025</v>
@@ -2559,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
         <f t="shared" si="3"/>
         <v>43026</v>
@@ -2580,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
         <f t="shared" si="3"/>
         <v>43027</v>
@@ -2601,27 +2282,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40">
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="37">
         <f t="shared" si="3"/>
         <v>43028</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="38">
         <f t="shared" si="0"/>
         <v>43028</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="39">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
         <f t="shared" si="3"/>
         <v>43029</v>
@@ -2643,7 +2331,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="16">
         <f t="shared" si="3"/>
         <v>43030</v>
@@ -2665,7 +2353,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="16">
         <f t="shared" si="3"/>
         <v>43031</v>
@@ -2686,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
         <f t="shared" si="3"/>
         <v>43032</v>
@@ -2707,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="16">
         <f t="shared" si="3"/>
         <v>43033</v>
@@ -2728,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="16">
         <f t="shared" si="3"/>
         <v>43034</v>
@@ -2749,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="16">
         <f t="shared" si="3"/>
         <v>43035</v>
@@ -2770,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="16">
         <f t="shared" si="3"/>
         <v>43036</v>
@@ -2792,7 +2480,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="16">
         <f t="shared" si="3"/>
         <v>43037</v>
@@ -2814,7 +2502,7 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
         <f t="shared" si="3"/>
         <v>43038</v>
@@ -2835,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <f t="shared" si="3"/>
         <v>43039</v>
@@ -2858,10 +2546,10 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="49"/>
       <c r="C33">
         <f>3*Zusammenfassung!B1</f>
         <v>27</v>
@@ -2869,91 +2557,106 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="20">
         <f>SUM(G2:G32)</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="H34" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D14:G14"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H21:K21"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="46" priority="22" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="54" priority="25" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G13 A22:G32 A21:D21 A15:G20 A14:D14">
-    <cfRule type="expression" dxfId="45" priority="21">
+  <conditionalFormatting sqref="A2:G13 A22:G32 A21:C21 A15:G20 A14:C14 G14 G21">
+    <cfRule type="expression" dxfId="53" priority="24">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="44" priority="11">
+    <cfRule type="expression" dxfId="52" priority="14">
       <formula>WEEKDAY($A8,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="43" priority="10">
+    <cfRule type="expression" dxfId="51" priority="13">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="42" priority="9">
+    <cfRule type="expression" dxfId="50" priority="12">
       <formula>WEEKDAY($A9,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="41" priority="8">
+    <cfRule type="expression" dxfId="49" priority="11">
       <formula>WEEKDAY($A15,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="40" priority="7">
+    <cfRule type="expression" dxfId="48" priority="10">
       <formula>WEEKDAY($A17,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="39" priority="6">
+    <cfRule type="expression" dxfId="47" priority="9">
       <formula>WEEKDAY($A16,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="38" priority="5">
+    <cfRule type="expression" dxfId="46" priority="8">
       <formula>WEEKDAY($A22,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="expression" dxfId="37" priority="4">
+    <cfRule type="expression" dxfId="45" priority="7">
       <formula>WEEKDAY($A23,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="36" priority="3">
+    <cfRule type="expression" dxfId="44" priority="6">
       <formula>WEEKDAY($A29,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="43" priority="5">
       <formula>WEEKDAY($A30,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="34" priority="1">
+    <cfRule type="expression" dxfId="42" priority="4">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>WEEKDAY($A14,2) &gt; 5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:F14">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>WEEKDAY($A14,2) &gt; 5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>WEEKDAY($A21,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.16" header="0" footer="0"/>
@@ -3347,24 +3050,24 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40">
+      <c r="A18" s="37">
         <f t="shared" si="3"/>
         <v>43056</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="45">
         <f t="shared" si="0"/>
         <v>43056</v>
       </c>
-      <c r="C18" s="52">
+      <c r="C18" s="46">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
@@ -3654,10 +3357,10 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="27">
         <f>5*Zusammenfassung!B1</f>
         <v>45</v>
@@ -3665,10 +3368,10 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
@@ -3687,57 +3390,57 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="33" priority="21" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="41" priority="21" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G17 A19:G32 A18:D18">
-    <cfRule type="expression" dxfId="32" priority="20">
+    <cfRule type="expression" dxfId="40" priority="20">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="31" priority="10">
+    <cfRule type="expression" dxfId="39" priority="10">
       <formula>WEEKDAY($A5,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="expression" dxfId="30" priority="9">
+    <cfRule type="expression" dxfId="38" priority="9">
       <formula>WEEKDAY($A6,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="29" priority="8">
+    <cfRule type="expression" dxfId="37" priority="8">
       <formula>WEEKDAY($A12,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="36" priority="7">
       <formula>WEEKDAY($A13,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="expression" dxfId="27" priority="6">
+    <cfRule type="expression" dxfId="35" priority="6">
       <formula>WEEKDAY($A19,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="26" priority="5">
+    <cfRule type="expression" dxfId="34" priority="5">
       <formula>WEEKDAY($A20,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="expression" dxfId="25" priority="4">
+    <cfRule type="expression" dxfId="33" priority="4">
       <formula>WEEKDAY($A26,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="32" priority="3">
       <formula>WEEKDAY($A27,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="31" priority="1">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4091,24 +3794,24 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40">
+      <c r="A16" s="37">
         <f t="shared" si="3"/>
         <v>43084</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="38">
         <f t="shared" si="0"/>
         <v>43084</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="39">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
@@ -4453,10 +4156,10 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="27">
         <f>4*Zusammenfassung!B1</f>
         <v>36</v>
@@ -4464,10 +4167,10 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
@@ -4486,62 +4189,62 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="22" priority="23" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="30" priority="23" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G15 A17:G32 A16:D16">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="29" priority="22">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>WEEKDAY($A25,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>WEEKDAY($A31,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="26" priority="9">
       <formula>WEEKDAY($A24,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="25" priority="8">
       <formula>WEEKDAY($A18,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="24" priority="7">
       <formula>WEEKDAY($A17,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>WEEKDAY($A11,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>WEEKDAY($A10,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>WEEKDAY($A4,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>WEEKDAY($A3,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4829,24 +4532,24 @@
       </c>
     </row>
     <row r="13" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40">
+      <c r="A13" s="37">
         <f t="shared" si="3"/>
         <v>43112</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13" s="38">
         <f t="shared" si="0"/>
         <v>43112</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="39">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
@@ -4977,24 +4680,24 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="40">
+      <c r="A20" s="37">
         <f t="shared" si="3"/>
         <v>43119</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="38">
         <f t="shared" si="0"/>
         <v>43119</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="39">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
@@ -5254,10 +4957,10 @@
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="27">
         <f>5*Zusammenfassung!B1</f>
         <v>45</v>
@@ -5265,10 +4968,10 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
@@ -5288,57 +4991,57 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="10" priority="13" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="18" priority="13" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G12 A21:G32 A20:D20 A14:G19 A13:D13">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>WEEKDAY($A8,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>WEEKDAY($A7,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="14" priority="8">
       <formula>WEEKDAY($A14,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>WEEKDAY($A15,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>WEEKDAY($A21,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>WEEKDAY($A22,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>WEEKDAY($A29,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>WEEKDAY($A28,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>